<commit_message>
mail favourite not fixed
</commit_message>
<xml_diff>
--- a/public/uploads/import_templates/Organizations Import Template.xlsx
+++ b/public/uploads/import_templates/Organizations Import Template.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA692D1-92E0-47E9-A8EB-B7106EE06EA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
@@ -32,12 +33,15 @@
   </si>
   <si>
     <t>Post Code</t>
+  </si>
+  <si>
+    <t>Emails</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -98,9 +102,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -138,9 +142,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -175,7 +179,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -210,7 +214,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -383,24 +387,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
-    <col min="3" max="3" width="30.140625" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="3" max="3" width="30.109375" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -419,8 +423,11 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2" s="1"/>
     </row>
   </sheetData>

</xml_diff>